<commit_message>
Se eleva el Trabajo POM finalizado
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/DatosExcel.xlsx
+++ b/src/test/resources/datos/DatosExcel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia.montes\Desktop\Clases Automation\Selenium\TrabajoPOM_MontesDeOca\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F70AB0-178B-47D1-A7F6-D4FCED0F62A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6842CD-65B0-4EFA-B755-ACC693D3A527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{517FF27C-4D4C-46CF-AB98-15510B62E25C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="604" xr2:uid="{517FF27C-4D4C-46CF-AB98-15510B62E25C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="DatosCP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,9 +63,6 @@
     <t>CP007_productoEscritorioMenu</t>
   </si>
   <si>
-    <t>CP008_productoArteMenu</t>
-  </si>
-  <si>
     <t>CP009_creacionCtaGorsh_MailExistente</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Organizador Multiuso Transparente</t>
   </si>
   <si>
-    <t>Cuadro Frases Papá</t>
-  </si>
-  <si>
     <t>maildeprueba29@noexite.com</t>
   </si>
   <si>
@@ -114,29 +108,43 @@
     <t>Usuario duplicado.</t>
   </si>
   <si>
+    <t>Clave incorrecta o no existe el usuario.</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>Ingrese una dirección de e-mail válida.</t>
+  </si>
+  <si>
+    <t>maildeprueba29</t>
+  </si>
+  <si>
+    <t>Vinilo Puerta Dragón</t>
+  </si>
+  <si>
+    <t>CP008_productoViniloMenu</t>
+  </si>
+  <si>
     <t>Prueba123</t>
-  </si>
-  <si>
-    <t>Clave incorrecta o no existe el usuario.</t>
-  </si>
-  <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>Ingrese una dirección de e-mail válida.</t>
-  </si>
-  <si>
-    <t>maildeprueba29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,15 +194,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,7 +527,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -561,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -572,10 +583,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -585,10 +596,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -598,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -609,7 +620,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -620,7 +631,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -628,10 +639,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -639,67 +650,70 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" display="maildeprueba29@" xr:uid="{75D01692-5A42-4C70-85F7-381093F04952}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>